<commit_message>
MAGMA-AUTO MIS AND BILLING OK
</commit_message>
<xml_diff>
--- a/media/SLICE/MIS/SLICE PERFORMANCE.xlsx
+++ b/media/SLICE/MIS/SLICE PERFORMANCE.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,16 +547,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12360176</v>
+        <v>12973319</v>
       </c>
       <c r="C2" t="n">
-        <v>248</v>
+        <v>277</v>
       </c>
       <c r="D2" t="n">
-        <v>132</v>
+        <v>215</v>
       </c>
       <c r="E2" t="n">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -568,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>5704206</v>
+        <v>10370416</v>
       </c>
       <c r="J2" t="n">
-        <v>6593806</v>
+        <v>2546642</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -580,13 +580,13 @@
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>62164</v>
+        <v>56261</v>
       </c>
       <c r="N2" t="n">
-        <v>46.15</v>
+        <v>79.94</v>
       </c>
       <c r="O2" t="n">
-        <v>53.35</v>
+        <v>19.63</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -595,16 +595,16 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="S2" t="n">
-        <v>53.35</v>
+        <v>19.63</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>2850049</v>
+        <v>1128903</v>
       </c>
     </row>
     <row r="3">
@@ -614,13 +614,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>657366</v>
+        <v>4619368</v>
       </c>
       <c r="C3" t="n">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="D3" t="n">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -629,13 +629,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I3" t="n">
-        <v>441432</v>
+        <v>4186884</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -644,13 +644,13 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>215934</v>
+        <v>280699</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>151785</v>
       </c>
       <c r="N3" t="n">
-        <v>67.15000000000001</v>
+        <v>90.64</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
@@ -659,19 +659,19 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>32.85</v>
+        <v>6.08</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>3.29</v>
       </c>
       <c r="S3" t="n">
-        <v>32.85</v>
+        <v>6.08</v>
       </c>
       <c r="T3" t="n">
-        <v>32.85</v>
+        <v>6.08</v>
       </c>
       <c r="U3" t="n">
-        <v>125936</v>
+        <v>231682</v>
       </c>
     </row>
     <row r="4">
@@ -681,131 +681,64 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>855342</v>
+        <v>1375085</v>
       </c>
       <c r="C4" t="n">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D4" t="n">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>793750</v>
+        <v>1262414</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>9970</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>61592</v>
+        <v>102701</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>92.8</v>
+        <v>91.81</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>7.2</v>
+        <v>7.47</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>7.2</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="T4" t="n">
-        <v>7.2</v>
+        <v>7.47</v>
       </c>
       <c r="U4" t="n">
-        <v>49681</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>BKT3</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>512212</v>
-      </c>
-      <c r="C5" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" t="n">
-        <v>9</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>500530</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>11682</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>97.72</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>2.28</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="n">
-        <v>2.28</v>
-      </c>
-      <c r="T5" t="n">
-        <v>2.28</v>
-      </c>
-      <c r="U5" t="n">
-        <v>2600</v>
+        <v>63254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>